<commit_message>
added new keywords "switch_to_default_content", "check_radio_chk_selected", "check_radio_chk_not_selected", "drag_drop", "hover_mouse"
</commit_message>
<xml_diff>
--- a/test_scripts/edge/QS001_testscript1.xlsx
+++ b/test_scripts/edge/QS001_testscript1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\edge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793F0C2E-2819-40DF-A764-A24ED9E71206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43F93F5-C393-42D9-B9E9-D809C42CD278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>open_browser</t>
   </si>
@@ -39,11 +39,6 @@
     <t>tc_desc</t>
   </si>
   <si>
-    <t>To verify if "Save as Draft" button saves the notification as draft during creation of a new notification.
-1.adldofo
-2. fldldfodo</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
@@ -62,16 +57,137 @@
     <t>step</t>
   </si>
   <si>
-    <t xml:space="preserve">Step is stepd foe flsof lldfoe </t>
-  </si>
-  <si>
-    <t>https://www.google.com</t>
-  </si>
-  <si>
-    <t>WhatisthisstepWhatisthisstepWhatisthisstepWhatisthisstepWhatisthisstepWhatisthisstepWhatisthisstepWhatisthisstep</t>
-  </si>
-  <si>
-    <t>TS001</t>
+    <t>To verify if the below:
+1. All checkboxes able to check.</t>
+  </si>
+  <si>
+    <t>Open the browser</t>
+  </si>
+  <si>
+    <t>The browser opens successfully</t>
+  </si>
+  <si>
+    <t>https://jqueryui.com/</t>
+  </si>
+  <si>
+    <t>Open the checkbox radio page</t>
+  </si>
+  <si>
+    <t>The checkbox radio page opens successfully</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>Checkboxradio link</t>
+  </si>
+  <si>
+    <t>checkbox_page_css</t>
+  </si>
+  <si>
+    <t>1radio</t>
+  </si>
+  <si>
+    <t>ny_radio_css</t>
+  </si>
+  <si>
+    <t>2radio</t>
+  </si>
+  <si>
+    <t>3radio</t>
+  </si>
+  <si>
+    <t>paris_radio_css</t>
+  </si>
+  <si>
+    <t>london_radio_css</t>
+  </si>
+  <si>
+    <t>switch_to_iframe</t>
+  </si>
+  <si>
+    <t>iframe</t>
+  </si>
+  <si>
+    <t>checkbox_iframe_css</t>
+  </si>
+  <si>
+    <t>checkbox_no_icons_link_css</t>
+  </si>
+  <si>
+    <t>checkboxnoicons link</t>
+  </si>
+  <si>
+    <t>1check</t>
+  </si>
+  <si>
+    <t>2star_check_css</t>
+  </si>
+  <si>
+    <t>2check</t>
+  </si>
+  <si>
+    <t>3check</t>
+  </si>
+  <si>
+    <t>4check</t>
+  </si>
+  <si>
+    <t>3star_check_css</t>
+  </si>
+  <si>
+    <t>4star_check_css</t>
+  </si>
+  <si>
+    <t>5star_check_css</t>
+  </si>
+  <si>
+    <t>Click on no icons link</t>
+  </si>
+  <si>
+    <t>The no icons page opens successfully</t>
+  </si>
+  <si>
+    <t>Click on all radio buttons anc check</t>
+  </si>
+  <si>
+    <t>Should be able to click on each radio button and that button is selected</t>
+  </si>
+  <si>
+    <t>Click on all check boxes anc check</t>
+  </si>
+  <si>
+    <t>Should be able to click on all check boxes and all should be checked.</t>
+  </si>
+  <si>
+    <t>QS001</t>
+  </si>
+  <si>
+    <t>check_radio_chk_selected</t>
+  </si>
+  <si>
+    <t>check_radio_chk_not_selected</t>
+  </si>
+  <si>
+    <t>ny_radio1_css</t>
+  </si>
+  <si>
+    <t>london_radio1_css</t>
+  </si>
+  <si>
+    <t>paris_radio1_css</t>
+  </si>
+  <si>
+    <t>2star_check1_css</t>
+  </si>
+  <si>
+    <t>3star_check1_css</t>
+  </si>
+  <si>
+    <t>4star_check1_css</t>
+  </si>
+  <si>
+    <t>5star_check1_css</t>
   </si>
 </sst>
 </file>
@@ -122,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -133,6 +249,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,15 +567,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3916CC0C-2E25-4DCF-A97F-45AF0FE46343}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.77734375" customWidth="1"/>
@@ -464,16 +583,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -481,26 +600,26 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -509,10 +628,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,47 +639,298 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D24" s="5"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="4"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D28" s="4"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D30" s="4"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D32" s="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" s="5"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D36" s="4"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D38" s="4"/>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="4"/>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="4"/>
     </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="5"/>
+    </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="5"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="4"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>